<commit_message>
Make a leaflet map
</commit_message>
<xml_diff>
--- a/output/extraction_selection.xlsx
+++ b/output/extraction_selection.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Analysis\5_Coastwide\Multispecies\Alaska Hatchery Research Program\PWS-Pink-WGR\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krshedd\R\PWS-Pink-WGR\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FF0C69-93F0-41BC-841B-6F8010A4B9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D34E36-C995-455C-AB15-969696462F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{FA798E47-A574-4989-80DD-0EB43D2732B0}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{A645C391-7544-40B5-A5EC-18E970720C67}"/>
   </bookViews>
   <sheets>
     <sheet name="background" sheetId="3" r:id="rId1"/>
@@ -43,6 +42,406 @@
     <author>Shedd, Kyle R (DFG)</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B6AC0B21-7718-4AF7-8098-5B02F091355B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Reference to Table 1 of the contract with Purdue that lays out the study design.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{CCC645C8-E3AF-4512-926B-074DE97F0EEE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Reference to Table 1 of the contract with Purdue that lays out the study design.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{3B6D609A-631C-439A-A998-8164E762205E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+hatchery = hatchery broodstock sample
+source = brood source population (i.e. wild population used to develop the hatchery broodstock, however, in some instances we don't have samples from the exact population, so we used the nearest population from which we have samples)
+wild = no thermal-otolith mark, natural-origin fish, but may have hatchery ancestry in prior generations
+stray = thermal-otolith mark present, a hatchery-origin fish that strayed into a natural stream and died there.
+All samples from objective B were collected from post-spawn carcasses.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{615FB6AD-EBCC-4B88-A6AD-8F4372990801}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Location of collection
+AFK = Armin F. Koernig hatchery located on Evan's Island in Southwestern PWS near the village of Chenega, operated by Prince William Sound Aquaculture Association (PWSAC)
+Cannery Creek = hatchery located on Cannery Creek in Unakwik Inlet in Northern PWS, operated by PWSAC
+VFDA = Valdez Fisheries Development Association (VFDA) which runs the Solomon Gulch hatchery in Northeastern PWS near Valdez</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{180878AE-B931-463A-86DC-2CD700659D90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+finer scale information on where each collection came from
+egg take = within the hatchery during spawning (i.e. stripping of eggs and milt from broodstock)
+middle tidal = within the intertidal zone
+early upstream = early-run (relative to the stream), upstream of any intertidal influence, strictly freshwater
+late upstream = late-run (relative to the stream), upstream of any intertidal influence, strictly freshwater
+upstream and intertidal = we have data on where individual fish were collected, some were collected in the intertidal zone, others in upstream habitat (i.e., freshwater, above tidal influence), see the "individuals" tab for details
+upstream = all fish were collected above tidal influence in freshwater habitat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{6FA66307-2F5B-4B4E-95AB-1F80727A584A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Do individual fish have paired sex data?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{67DF9C99-E852-482E-A4D7-D834B0324D74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Do individual fish or collections have paired sample date data? This is important because sometimes we see stock structure based on run timing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{59BDA63E-0F51-4AF2-AFC4-83F95679A862}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Alaskan hatcheries did not start using thermal otolith marks to identify hatchery-origin fish until 1991, with 100% otolith marking of PWS pink salmon not achieved until brood year 1995 (fish returning in 1997). Prior to universal thermal otolith marking, there was no way to determine if pink salmon sampled in a stream were "wild" or hatchery strays. Thus, all of the historical, source populations may have some unkown number of hatchery strays mixed in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{CCCF1B24-E569-423F-98E3-A7B48D8A493A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Even-year lineage or odd-year lineage?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3BA7C31A-9B9B-41F9-8C0B-BF1BA5B42E78}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+historical vs. contemporary as defined in Table 1 of the contract laying out the study design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{53542191-86E6-4DDC-91D4-B4AC0ABDED37}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Collection year (not brood year!)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{D45C4320-D2DB-458F-AA26-A2B5932A27B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ADF&amp;G's internal collection code, SILLY is an acronym that stands for Species, Identifier, Location, Location, Year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{F704519F-B5E3-4959-800F-0F15DE557577}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Collection level, not fish level, for mapping purposes only</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{87CB7415-B10D-40EF-A08A-00B212ADE90D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Collection level, not fish level, for mapping purposes only</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{C99435E3-4499-4AF7-8266-3412BED7EFA8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+how many samples in this collection?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{A027A975-E882-4094-BFB2-C1A11A24CAFA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+any other notes that I could find in our database, some of our older collections are lacking in data
+LOKI = ADF&amp;G genetics database name
+AWC = anadramous waters catalog number (https://www.adfg.alaska.gov/sf/SARR/AWC/index.cfm?ADFG=main.interactive), this is a great resource for distinguishing among streams in Alaska (there are a LOT of "Fish Creek" locations, but each has their own, unique AWC number
+for the objective B , wild collections, since we only know origin information from the presence/absence of thermal otoltih marks, but those do not tell us ancestry (i.e., the offspring of two hatchery strays will not have a thermal otolith mark, and is thus a "natural-origin" fish), I attempted to use our pedigree data to find natural-origin fish that had at least 1 natural-origin parent to help avoid natural-origin fish with hatchery ancestry in previous generations. our pedigrees are very sparse, so this is the best I could do.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F2" authorId="0" shapeId="0" xr:uid="{D6181F76-2CC3-41C7-BBB6-78FEF95E177B}">
       <text>
         <r>
@@ -119,8 +518,168 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Shedd, Kyle R (DFG)</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2581CCE2-936E-4F50-B854-B9369365A881}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ADF&amp;G internal collection code
+SILLY is an acronym that stands for
+Species
+Identifier
+Location
+Location
+Year (2 digits)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5DE602A6-CE85-4B5A-965C-B5FDB401A211}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ADF&amp;G internal fish identifier within an collection</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9220758B-6D2C-40CF-9D9D-5DC1AB358FD3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sex, if known was determined either from secondary sexual characteristics or visual examination of gamets (eggs or milt)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3B7BC303-1167-455E-9AB0-AC0A1BD955E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+as determined by the presence or absence of thermal otolith marks</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{B15C5B3D-ED23-4CBE-A09D-5FBB184AB521}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+collection date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D1A59034-C503-4331-A947-49945E205073}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shedd, Kyle R (DFG):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+any other information on these fish or the collection</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3192" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3194" uniqueCount="108">
   <si>
     <t>silly</t>
   </si>
@@ -438,6 +997,12 @@
   </si>
   <si>
     <t>late tidal</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
   </si>
 </sst>
 </file>
@@ -900,9 +1465,8 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -914,19 +1478,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360DF842-2B23-40F7-9349-B361965D9C45}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
@@ -936,11 +1499,12 @@
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="167" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="167" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -978,13 +1542,19 @@
         <v>0</v>
       </c>
       <c r="M1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1021,14 +1591,20 @@
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
+        <v>60.7988</v>
+      </c>
+      <c r="N2" s="4">
+        <v>-148.08590000000001</v>
+      </c>
+      <c r="O2">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1065,14 +1641,20 @@
       <c r="L3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
+        <v>60.065429999999999</v>
+      </c>
+      <c r="N3" s="4">
+        <v>-148.06542999999999</v>
+      </c>
+      <c r="O3">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1109,14 +1691,20 @@
       <c r="L4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
+        <v>60.7988</v>
+      </c>
+      <c r="N4" s="4">
+        <v>-148.08590000000001</v>
+      </c>
+      <c r="O4">
         <v>36</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1153,14 +1741,20 @@
       <c r="L5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="4">
+        <v>60.051116999999998</v>
+      </c>
+      <c r="N5" s="4">
+        <v>-148.06540000000001</v>
+      </c>
+      <c r="O5">
         <v>36</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1197,14 +1791,20 @@
       <c r="L6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="4">
+        <v>61.018720000000002</v>
+      </c>
+      <c r="N6" s="4">
+        <v>-147.51437999999999</v>
+      </c>
+      <c r="O6">
         <v>36</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1241,14 +1841,20 @@
       <c r="L7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="4">
+        <v>61.014800000000001</v>
+      </c>
+      <c r="N7" s="4">
+        <v>-147.51859999999999</v>
+      </c>
+      <c r="O7">
         <v>36</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1285,14 +1891,20 @@
       <c r="L8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="4">
+        <v>61.018720000000002</v>
+      </c>
+      <c r="N8" s="4">
+        <v>-147.51437999999999</v>
+      </c>
+      <c r="O8">
         <v>36</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1329,14 +1941,20 @@
       <c r="L9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
+        <v>61.0837</v>
+      </c>
+      <c r="N9" s="4">
+        <v>-146.30539999999999</v>
+      </c>
+      <c r="O9">
         <v>36</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1373,14 +1991,20 @@
       <c r="L10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
+        <v>61.130800000000001</v>
+      </c>
+      <c r="N10" s="4">
+        <v>-146.34829999999999</v>
+      </c>
+      <c r="O10">
         <v>36</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1417,14 +2041,20 @@
       <c r="L11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
+        <v>61.0837</v>
+      </c>
+      <c r="N11" s="4">
+        <v>-146.30539999999999</v>
+      </c>
+      <c r="O11">
         <v>36</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1461,14 +2091,20 @@
       <c r="L12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="4">
+        <v>61.130800000000001</v>
+      </c>
+      <c r="N12" s="4">
+        <v>-146.34829999999999</v>
+      </c>
+      <c r="O12">
         <v>36</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1505,14 +2141,20 @@
       <c r="L13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
+        <v>60.941899999999997</v>
+      </c>
+      <c r="N13" s="4">
+        <v>-146.56569999999999</v>
+      </c>
+      <c r="O13">
         <v>36</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1549,14 +2191,20 @@
       <c r="L14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="4">
+        <v>60.940055000000001</v>
+      </c>
+      <c r="N14" s="4">
+        <v>-146.56462300000001</v>
+      </c>
+      <c r="O14">
         <v>18</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1593,14 +2241,20 @@
       <c r="L15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="4">
+        <v>60.941634999999998</v>
+      </c>
+      <c r="N15" s="4">
+        <v>-146.566213</v>
+      </c>
+      <c r="O15">
         <v>18</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1637,14 +2291,20 @@
       <c r="L16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="4">
+        <v>60.377000000000002</v>
+      </c>
+      <c r="N16" s="4">
+        <v>-148.1515</v>
+      </c>
+      <c r="O16">
         <v>18</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1682,13 +2342,19 @@
         <v>57</v>
       </c>
       <c r="M17" s="4">
+        <v>60.377000000000002</v>
+      </c>
+      <c r="N17" s="4">
+        <v>-148.1515</v>
+      </c>
+      <c r="O17">
         <v>18</v>
       </c>
-      <c r="N17" t="s">
+      <c r="P17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1725,14 +2391,20 @@
       <c r="L18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="4">
+        <v>60.377299999999998</v>
+      </c>
+      <c r="N18" s="4">
+        <v>-148.15039999999999</v>
+      </c>
+      <c r="O18">
         <v>36</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1766,14 +2438,20 @@
       <c r="L19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="4">
+        <v>61.018999999999998</v>
+      </c>
+      <c r="N19" s="4">
+        <v>-146.60499999999999</v>
+      </c>
+      <c r="O19">
         <v>36</v>
       </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1810,14 +2488,20 @@
       <c r="L20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="4">
+        <v>61.019542000000001</v>
+      </c>
+      <c r="N20" s="4">
+        <v>-146.60724500000001</v>
+      </c>
+      <c r="O20">
         <v>18</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1854,14 +2538,20 @@
       <c r="L21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="4">
+        <v>61.019188999999997</v>
+      </c>
+      <c r="N21" s="4">
+        <v>-146.605133</v>
+      </c>
+      <c r="O21">
         <v>18</v>
       </c>
-      <c r="N21" t="s">
+      <c r="P21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1898,14 +2588,20 @@
       <c r="L22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="4">
+        <v>60.941899999999997</v>
+      </c>
+      <c r="N22" s="4">
+        <v>-146.56569999999999</v>
+      </c>
+      <c r="O22">
         <v>36</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1942,14 +2638,20 @@
       <c r="L23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="4">
+        <v>60.941313000000001</v>
+      </c>
+      <c r="N23" s="4">
+        <v>-146.56613200000001</v>
+      </c>
+      <c r="O23">
         <v>36</v>
       </c>
-      <c r="N23" t="s">
+      <c r="P23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1986,14 +2688,20 @@
       <c r="L24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="4">
+        <v>60.302100000000003</v>
+      </c>
+      <c r="N24" s="4">
+        <v>-147.18199999999999</v>
+      </c>
+      <c r="O24">
         <v>36</v>
       </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2030,14 +2738,20 @@
       <c r="L25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="4">
+        <v>60.302100000000003</v>
+      </c>
+      <c r="N25" s="4">
+        <v>-147.18199999999999</v>
+      </c>
+      <c r="O25">
         <v>36</v>
       </c>
-      <c r="N25" t="s">
+      <c r="P25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2074,14 +2788,20 @@
       <c r="L26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="4">
+        <v>60.302100000000003</v>
+      </c>
+      <c r="N26" s="4">
+        <v>-147.18199999999999</v>
+      </c>
+      <c r="O26">
         <v>36</v>
       </c>
-      <c r="N26" t="s">
+      <c r="P26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2118,14 +2838,20 @@
       <c r="L27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="4">
+        <v>60.302100000000003</v>
+      </c>
+      <c r="N27" s="4">
+        <v>-147.18199999999999</v>
+      </c>
+      <c r="O27">
         <v>36</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2162,14 +2888,20 @@
       <c r="L28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="4">
+        <v>60.208599999999997</v>
+      </c>
+      <c r="N28" s="4">
+        <v>-147.762</v>
+      </c>
+      <c r="O28">
         <v>36</v>
       </c>
-      <c r="N28" t="s">
+      <c r="P28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2206,14 +2938,20 @@
       <c r="L29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="4">
+        <v>60.208599999999997</v>
+      </c>
+      <c r="N29" s="4">
+        <v>-147.762</v>
+      </c>
+      <c r="O29">
         <v>36</v>
       </c>
-      <c r="N29" t="s">
+      <c r="P29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2250,14 +2988,20 @@
       <c r="L30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="4">
+        <v>60.208599999999997</v>
+      </c>
+      <c r="N30" s="4">
+        <v>-147.762</v>
+      </c>
+      <c r="O30">
         <v>36</v>
       </c>
-      <c r="N30" t="s">
+      <c r="P30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2294,14 +3038,20 @@
       <c r="L31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="4">
+        <v>60.208599999999997</v>
+      </c>
+      <c r="N31" s="4">
+        <v>-147.762</v>
+      </c>
+      <c r="O31">
         <v>36</v>
       </c>
-      <c r="N31" t="s">
+      <c r="P31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2338,14 +3088,20 @@
       <c r="L32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="4">
+        <v>60.642899999999997</v>
+      </c>
+      <c r="N32" s="4">
+        <v>-145.81309999999999</v>
+      </c>
+      <c r="O32">
         <v>36</v>
       </c>
-      <c r="N32" t="s">
+      <c r="P32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -2382,10 +3138,16 @@
       <c r="L33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="4">
+        <v>60.642899999999997</v>
+      </c>
+      <c r="N33" s="4">
+        <v>-145.81309999999999</v>
+      </c>
+      <c r="O33">
         <v>36</v>
       </c>
-      <c r="N33" t="s">
+      <c r="P33" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2398,15 +3160,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4FA352-7A93-4E0D-A700-9E8770B1B27B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4FA352-7A93-4E0D-A700-9E8770B1B27B}">
   <dimension ref="A1:F1045"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19243,5 +20002,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>